<commit_message>
Zweite Seite für Vergleich
</commit_message>
<xml_diff>
--- a/daten/population_ch.xlsx
+++ b/daten/population_ch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/laurazanchin/Dropbox/Mac/Desktop/master/daten/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B8F814C-720C-FB4C-8502-DCC50CB51BEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB01970A-C822-6A46-8903-0E52AEB49363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="1060" windowWidth="33200" windowHeight="17940" xr2:uid="{752BF075-A2E0-0249-B13B-E08598446618}"/>
+    <workbookView xWindow="400" yWindow="1060" windowWidth="33200" windowHeight="17940" xr2:uid="{752BF075-A2E0-0249-B13B-E08598446618}"/>
   </bookViews>
   <sheets>
     <sheet name="Kanton" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4673" uniqueCount="4661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4673" uniqueCount="4663">
   <si>
     <t>ZH</t>
   </si>
@@ -14024,13 +14024,19 @@
   </si>
   <si>
     <t>Nummer</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>anzahl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -14050,6 +14056,25 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -14073,7 +14098,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -14081,6 +14106,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -14398,7 +14426,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14407,299 +14435,299 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>331</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>333</v>
+      <c r="B1" s="5" t="s">
+        <v>4661</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>4662</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="7">
         <v>1564662</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="7">
         <v>1047473</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="7">
         <v>420326</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="7">
         <v>37047</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6" s="7">
         <v>163689</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="7">
         <v>38435</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="7">
         <v>43894</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="7">
         <v>41190</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="7">
         <v>129787</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="7">
         <v>329809</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="7">
         <v>280245</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="7">
         <v>196036</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="7">
         <v>292817</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="7">
         <v>83995</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="7">
         <v>55585</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="7">
         <v>16360</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="7">
         <v>519245</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="7">
         <v>201376</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="7">
         <v>703086</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="3">
+      <c r="C21" s="7">
         <v>285964</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C22" s="7">
         <v>352181</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C23" s="7">
         <v>822968</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="3">
+      <c r="C24" s="7">
         <v>353209</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="C25" s="3">
+      <c r="C25" s="7">
         <v>176166</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C26" s="3">
+      <c r="C26" s="7">
         <v>509448</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="3">
+      <c r="C27" s="7">
         <v>73798</v>
       </c>
     </row>

</xml_diff>